<commit_message>
contains csv for adding to queue
</commit_message>
<xml_diff>
--- a/Week-6/REFWDemo/Data/Config.xlsx
+++ b/Week-6/REFWDemo/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Batches\220425-UiPath\Demo\REFWDemo\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Batches\230206-UiPath-BNYM\Trainer-Code\Week-6\REFWDemo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2620E627-70F2-4721-98CD-1F169BA6620C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA11596A-531C-4AC4-9B2F-09CF76644DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,7 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>BarbeQueue</t>
+    <t>Product_Queue</t>
   </si>
 </sst>
 </file>
@@ -174,10 +174,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -500,7 +500,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>